<commit_message>
manual add alt SN
</commit_message>
<xml_diff>
--- a/serialNumbers.xlsx
+++ b/serialNumbers.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,98 +424,24 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>20UPIDP9000007</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>101</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>20UPIDP9000008</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
-          <t>U</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>102</t>
         </is>
       </c>
     </row>

</xml_diff>